<commit_message>
- Updated RitualZones to 1.2.1 - RitualZones now has less lua overhead usage and a memory leak fixed
</commit_message>
<xml_diff>
--- a/RitualZones/scripts/mods/RitualZones/cache/TEST_TRACKER.xlsx
+++ b/RitualZones/scripts/mods/RitualZones/cache/TEST_TRACKER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SteamLibrary\steamapps\common\Warhammer 40,000 DARKTIDE\mods\RitualZones\scripts\mods\RitualZones\cache\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC94194-8E72-4F94-91D0-709E0BAB4B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2424B20B-7160-4A3E-B331-552AC5935CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{BE9A7E75-63AD-4948-BE56-2702377DBAFE}"/>
   </bookViews>
@@ -771,7 +771,7 @@
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -999,6 +999,7 @@
         <v>1461.00427246093</v>
       </c>
       <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" t="s">
@@ -1023,9 +1024,6 @@
         <v>1213.90515136718</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" t="s">

</xml_diff>